<commit_message>
[taekwon] enum 내 타겟 타입 추가
</commit_message>
<xml_diff>
--- a/GameData/Excel/enum.xlsx
+++ b/GameData/Excel/enum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\문서\GitHub\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6DEF21-B2EB-4039-9051-27CE66A8F3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3DD764-3DC2-4C50-8926-49C2E3499C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11736" yWindow="4740" windowWidth="34560" windowHeight="18792" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="11730" yWindow="4740" windowWidth="34560" windowHeight="18795" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="enum" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="125">
   <si>
     <t>int</t>
   </si>
@@ -341,18 +330,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ally</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>적</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>내자신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#전투 관련 - 몬스터 타입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -478,6 +459,30 @@
   </si>
   <si>
     <t>대미지류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ally_hp_lowest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ally_hp_highest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나 자신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력이 가장 높은 아군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력이 가장 낮은 아군</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -624,9 +629,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -664,7 +669,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -770,7 +775,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -912,7 +917,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -920,24 +925,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="3" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.19921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.59765625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.69921875" style="3"/>
+    <col min="5" max="5" width="40.625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -954,7 +959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -969,7 +974,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -984,7 +989,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="5" customFormat="1" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -993,7 +998,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1020,7 +1025,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1038,7 +1043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1056,21 +1061,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1080,15 +1085,15 @@
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1098,15 +1103,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1116,24 +1121,24 @@
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1143,15 +1148,15 @@
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1161,24 +1166,24 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1188,15 +1193,15 @@
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1206,24 +1211,24 @@
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" ref="C20:C28" si="1">UPPER(A20)&amp;"_"&amp;UPPER(B20)</f>
@@ -1233,15 +1238,15 @@
         <v>0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1251,24 +1256,24 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1278,12 +1283,12 @@
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>24</v>
@@ -1296,12 +1301,12 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>27</v>
@@ -1314,12 +1319,12 @@
         <v>2</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>28</v>
@@ -1332,15 +1337,15 @@
         <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1350,15 +1355,15 @@
         <v>4</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1368,10 +1373,10 @@
         <v>5</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>21</v>
       </c>
@@ -1380,7 +1385,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +1403,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>22</v>
       </c>
@@ -1416,7 +1421,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
@@ -1434,7 +1439,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
@@ -1452,7 +1457,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>22</v>
       </c>
@@ -1470,7 +1475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1493,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>22</v>
       </c>
@@ -1506,7 +1511,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>22</v>
       </c>
@@ -1524,7 +1529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1547,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
@@ -1560,7 +1565,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
@@ -1596,7 +1601,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>22</v>
       </c>
@@ -1614,7 +1619,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>22</v>
       </c>
@@ -1632,7 +1637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
@@ -1650,7 +1655,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>22</v>
       </c>
@@ -1668,7 +1673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>22</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>22</v>
       </c>
@@ -1722,7 +1727,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
@@ -1740,7 +1745,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>22</v>
       </c>
@@ -1758,7 +1763,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>22</v>
       </c>
@@ -1776,7 +1781,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>22</v>
       </c>
@@ -1794,7 +1799,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>22</v>
       </c>
@@ -1812,7 +1817,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>22</v>
       </c>
@@ -1830,7 +1835,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>22</v>
       </c>
@@ -1848,7 +1853,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>22</v>
       </c>
@@ -1884,7 +1889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>22</v>
       </c>
@@ -1902,7 +1907,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>82</v>
       </c>
@@ -1911,25 +1916,25 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="C60" s="1" t="str">
         <f t="shared" ref="C60" si="2">UPPER(A60)&amp;"_"&amp;UPPER(B60)</f>
-        <v>TARGET_TYPE_ALLY</v>
+        <v>TARGET_TYPE_SELF</v>
       </c>
       <c r="D60" s="3">
         <v>0</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>81</v>
       </c>
@@ -1937,14 +1942,50 @@
         <v>83</v>
       </c>
       <c r="C61" s="1" t="str">
-        <f t="shared" ref="C61" si="3">UPPER(A61)&amp;"_"&amp;UPPER(B61)</f>
+        <f t="shared" ref="C61:C62" si="3">UPPER(A61)&amp;"_"&amp;UPPER(B61)</f>
         <v>TARGET_TYPE_ENEMY</v>
       </c>
       <c r="D61" s="3">
         <v>1</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>TARGET_TYPE_ALLY_HP_HIGHEST</v>
+      </c>
+      <c r="D62" s="3">
+        <v>2</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="1" t="str">
+        <f t="shared" ref="C63" si="4">UPPER(A63)&amp;"_"&amp;UPPER(B63)</f>
+        <v>TARGET_TYPE_ALLY_HP_LOWEST</v>
+      </c>
+      <c r="D63" s="3">
+        <v>3</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[yerim] 도트 amorup 구현
</commit_message>
<xml_diff>
--- a/GameData/Excel/enum.xlsx
+++ b/GameData/Excel/enum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yerim\portfolio_Game\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76142320-21BE-4BEC-9397-8C6FAAEC03C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7203E606-C04E-4E51-83B3-B562F9D263F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18072" yWindow="5916" windowWidth="25740" windowHeight="13572" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="enum" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="202">
   <si>
     <t>int</t>
   </si>
@@ -760,6 +760,14 @@
   </si>
   <si>
     <t>보상 타입 - 재화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dot_amor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지속 방어도 획득</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1202,24 +1210,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.59765625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.69921875" style="3"/>
+    <col min="5" max="5" width="40.625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -1236,7 +1244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1251,7 +1259,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1266,7 +1274,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="5" customFormat="1" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1275,7 +1283,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1291,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f t="shared" ref="C5:C64" si="0">UPPER(A5)&amp;"_"&amp;UPPER(B5)</f>
+        <f t="shared" ref="C5:C65" si="0">UPPER(A5)&amp;"_"&amp;UPPER(B5)</f>
         <v>LANGUAGE_TYPE_KOR</v>
       </c>
       <c r="D5" s="1">
@@ -1293,7 +1301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1302,7 +1310,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1328,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1338,7 +1346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>84</v>
       </c>
@@ -1347,7 +1355,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>85</v>
       </c>
@@ -1365,7 +1373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>85</v>
       </c>
@@ -1383,7 +1391,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
@@ -1401,7 +1409,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>92</v>
       </c>
@@ -1410,7 +1418,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>94</v>
       </c>
@@ -1428,7 +1436,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>94</v>
       </c>
@@ -1446,7 +1454,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
@@ -1455,7 +1463,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>95</v>
       </c>
@@ -1473,7 +1481,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>95</v>
       </c>
@@ -1491,7 +1499,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>105</v>
       </c>
@@ -1500,7 +1508,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>104</v>
       </c>
@@ -1518,7 +1526,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>104</v>
       </c>
@@ -1536,7 +1544,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>107</v>
       </c>
@@ -1545,7 +1553,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>108</v>
       </c>
@@ -1563,7 +1571,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>108</v>
       </c>
@@ -1581,7 +1589,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>108</v>
       </c>
@@ -1599,7 +1607,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>108</v>
       </c>
@@ -1617,7 +1625,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>108</v>
       </c>
@@ -1635,7 +1643,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>108</v>
       </c>
@@ -1653,7 +1661,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1662,7 +1670,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
@@ -1680,7 +1688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -1698,7 +1706,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
@@ -1716,7 +1724,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
@@ -1734,7 +1742,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>21</v>
       </c>
@@ -1752,7 +1760,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1778,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>21</v>
       </c>
@@ -1788,7 +1796,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>21</v>
       </c>
@@ -1806,7 +1814,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -1824,7 +1832,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1850,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>21</v>
       </c>
@@ -1860,7 +1868,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
@@ -1878,7 +1886,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
@@ -1896,7 +1904,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -1914,7 +1922,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>21</v>
       </c>
@@ -1932,7 +1940,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>21</v>
       </c>
@@ -1950,7 +1958,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>21</v>
       </c>
@@ -1968,7 +1976,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>21</v>
       </c>
@@ -1986,7 +1994,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>21</v>
       </c>
@@ -2004,7 +2012,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>21</v>
       </c>
@@ -2022,7 +2030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>21</v>
       </c>
@@ -2040,7 +2048,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>21</v>
       </c>
@@ -2058,7 +2066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>21</v>
       </c>
@@ -2076,7 +2084,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2102,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>21</v>
       </c>
@@ -2112,7 +2120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>21</v>
       </c>
@@ -2130,7 +2138,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>21</v>
       </c>
@@ -2148,7 +2156,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>21</v>
       </c>
@@ -2166,7 +2174,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>21</v>
       </c>
@@ -2184,678 +2192,696 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>EFFECT_TYPE_DOT_AMOR</v>
+      </c>
+      <c r="D59" s="3">
+        <v>29</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>SUPPORT_MODULE_EFFECT_REDUCE_PRODUCT_AP</v>
-      </c>
-      <c r="D60" s="3">
-        <v>0</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>SUPPORT_MODULE_EFFECT_INCREASE_PRODUCT_AP</v>
+        <v>SUPPORT_MODULE_EFFECT_REDUCE_PRODUCT_AP</v>
       </c>
       <c r="D61" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>SUPPORT_MODULE_EFFECT_REDUCE_PRODUCT_VALUE</v>
+        <v>SUPPORT_MODULE_EFFECT_INCREASE_PRODUCT_AP</v>
       </c>
       <c r="D62" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>SUPPORT_MODULE_EFFECT_INCREASE_PRODUCT_VALUE</v>
+        <v>SUPPORT_MODULE_EFFECT_REDUCE_PRODUCT_VALUE</v>
       </c>
       <c r="D63" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>SUPPORT_MODULE_EFFECT_INCREASE_PRODUCT_VALUE</v>
+      </c>
+      <c r="D64" s="3">
+        <v>3</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="1" t="str">
+      <c r="C65" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SUPPORT_MODULE_EFFECT_CHANGE_PRODUCT_SPELL</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D65" s="3">
         <v>4</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+    <row r="66" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C66" s="1" t="str">
-        <f t="shared" ref="C66" si="2">UPPER(A66)&amp;"_"&amp;UPPER(B66)</f>
-        <v>TARGET_TYPE_SELF</v>
-      </c>
-      <c r="D66" s="3">
-        <v>0</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="C67" s="1" t="str">
-        <f t="shared" ref="C67:C68" si="3">UPPER(A67)&amp;"_"&amp;UPPER(B67)</f>
-        <v>TARGET_TYPE_ENEMY</v>
+        <f t="shared" ref="C67" si="2">UPPER(A67)&amp;"_"&amp;UPPER(B67)</f>
+        <v>TARGET_TYPE_SELF</v>
       </c>
       <c r="D67" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="1" t="str">
+        <f t="shared" ref="C68:C69" si="3">UPPER(A68)&amp;"_"&amp;UPPER(B68)</f>
+        <v>TARGET_TYPE_ENEMY</v>
+      </c>
+      <c r="D68" s="3">
+        <v>1</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="1" t="str">
+      <c r="C69" s="1" t="str">
         <f t="shared" si="3"/>
         <v>TARGET_TYPE_ALLY_HP_HIGHEST</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D69" s="3">
         <v>2</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C69" s="1" t="str">
-        <f t="shared" ref="C69" si="4">UPPER(A69)&amp;"_"&amp;UPPER(B69)</f>
+      <c r="C70" s="1" t="str">
+        <f t="shared" ref="C70" si="4">UPPER(A70)&amp;"_"&amp;UPPER(B70)</f>
         <v>TARGET_TYPE_ALLY_HP_LOWEST</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D70" s="3">
         <v>3</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
+    <row r="71" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C71" s="1" t="str">
-        <f t="shared" ref="C71:C74" si="5">UPPER(A71)&amp;"_"&amp;UPPER(B71)</f>
+      <c r="C72" s="1" t="str">
+        <f t="shared" ref="C72:C75" si="5">UPPER(A72)&amp;"_"&amp;UPPER(B72)</f>
         <v>ACTIVE_CONDITION_BATTLE_START</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D72" s="3">
         <v>0</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C72" s="1" t="str">
+      <c r="C73" s="1" t="str">
         <f t="shared" si="5"/>
         <v>ACTIVE_CONDITION_BATTLE_END</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D73" s="3">
         <v>1</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C73" s="1" t="str">
+      <c r="C74" s="1" t="str">
         <f t="shared" si="5"/>
         <v>ACTIVE_CONDITION_HP_MINUS_VALUE</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D74" s="3">
         <v>2</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C74" s="1" t="str">
+      <c r="C75" s="1" t="str">
         <f t="shared" si="5"/>
         <v>ACTIVE_CONDITION_HP_PERCENT</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D75" s="3">
         <v>3</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C76" s="1" t="str">
-        <f t="shared" ref="C76:C77" si="6">UPPER(A76)&amp;"_"&amp;UPPER(B76)</f>
+      <c r="C77" s="1" t="str">
+        <f t="shared" ref="C77:C78" si="6">UPPER(A77)&amp;"_"&amp;UPPER(B77)</f>
         <v>RELIC_EFFECT_HEAL</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D77" s="3">
         <v>0</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C77" s="1" t="str">
+      <c r="C78" s="1" t="str">
         <f t="shared" si="6"/>
         <v>RELIC_EFFECT_ARMOR</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D78" s="3">
         <v>1</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
+    <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C79" s="1" t="str">
-        <f t="shared" ref="C79:C83" si="7">UPPER(A79)&amp;"_"&amp;UPPER(B79)</f>
-        <v>MAP_TYPE_BATTLE_NORMAL</v>
-      </c>
-      <c r="D79" s="3">
-        <v>0</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" s="1" t="str">
+        <f t="shared" ref="C80:C84" si="7">UPPER(A80)&amp;"_"&amp;UPPER(B80)</f>
+        <v>MAP_TYPE_BATTLE_NORMAL</v>
+      </c>
+      <c r="D80" s="3">
+        <v>0</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C80" s="1" t="str">
+      <c r="C81" s="1" t="str">
         <f t="shared" si="7"/>
         <v>MAP_TYPE_BATTLE_ELITE</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D81" s="3">
         <v>1</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C81" s="1" t="str">
+      <c r="C82" s="1" t="str">
         <f t="shared" si="7"/>
         <v>MAP_TYPE_BATTLE_BOSS</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D82" s="3">
         <v>2</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C82" s="1" t="str">
+      <c r="C83" s="1" t="str">
         <f t="shared" si="7"/>
         <v>MAP_TYPE_SHOP</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D83" s="3">
         <v>3</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C83" s="1" t="str">
+      <c r="C84" s="1" t="str">
         <f t="shared" si="7"/>
         <v>MAP_TYPE_ENHANCE</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D84" s="3">
         <v>4</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
+    <row r="85" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C85" s="1" t="str">
-        <f t="shared" ref="C85:C100" si="8">UPPER(A85)&amp;"_"&amp;UPPER(B85)</f>
-        <v>REWARD_TYPE_ITEM</v>
-      </c>
-      <c r="D85" s="3">
-        <v>0</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86" s="1" t="str">
+        <f t="shared" ref="C86:C101" si="8">UPPER(A86)&amp;"_"&amp;UPPER(B86)</f>
+        <v>REWARD_TYPE_ITEM</v>
+      </c>
+      <c r="D86" s="3">
+        <v>0</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C86" s="1" t="str">
+      <c r="C87" s="1" t="str">
         <f t="shared" si="8"/>
         <v>REWARD_TYPE_SPELL_SOURCE</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D87" s="3">
         <v>1</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E87" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C87" s="1" t="str">
+      <c r="C88" s="1" t="str">
         <f t="shared" si="8"/>
         <v>REWARD_TYPE_SUPPORT_MODULE</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D88" s="3">
         <v>2</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="1" t="str">
+      <c r="C89" s="1" t="str">
         <f t="shared" si="8"/>
         <v>REWARD_TYPE_MONEY</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D89" s="3">
         <v>3</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
+    <row r="90" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C90" s="1" t="str">
+      <c r="C91" s="1" t="str">
         <f t="shared" si="8"/>
         <v>EXCEPTION_TYPE_OWN_SPELL_SOURCE</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D91" s="3">
         <v>0</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E91" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C91" s="1" t="str">
+      <c r="C92" s="1" t="str">
         <f t="shared" si="8"/>
         <v>EXCEPTION_TYPE_NO_SPELL_SOURCE</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D92" s="3">
         <v>1</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C92" s="1" t="str">
+      <c r="C93" s="1" t="str">
         <f t="shared" si="8"/>
         <v>EXCEPTION_TYPE_CLEAR_MAP</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D93" s="3">
         <v>2</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C93" s="1" t="str">
+      <c r="C94" s="1" t="str">
         <f t="shared" si="8"/>
         <v>EXCEPTION_TYPE_NOT_CLEAR_MAP</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D94" s="3">
         <v>3</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
+    <row r="95" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C95" s="1" t="str">
+      <c r="C96" s="1" t="str">
         <f t="shared" si="8"/>
         <v>RARITY_NORMAL</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D96" s="3">
         <v>0</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C96" s="1" t="str">
+      <c r="C97" s="1" t="str">
         <f t="shared" si="8"/>
         <v>RARITY_RARE</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D97" s="3">
         <v>1</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B98" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C97" s="1" t="str">
+      <c r="C98" s="1" t="str">
         <f t="shared" si="8"/>
         <v>RARITY_EPIC</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D98" s="3">
         <v>2</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
+    <row r="99" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C99" s="1" t="str">
+      <c r="C100" s="1" t="str">
         <f t="shared" si="8"/>
         <v>LOGICAL_OPERATOR_AND</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D100" s="3">
         <v>0</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C100" s="1" t="str">
+      <c r="C101" s="1" t="str">
         <f t="shared" si="8"/>
         <v>LOGICAL_OPERATOR_OR</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D101" s="3">
         <v>1</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[yerim] target all  구현 완료
</commit_message>
<xml_diff>
--- a/GameData/Excel/enum.xlsx
+++ b/GameData/Excel/enum.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yerim\portfolio_Game\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7203E606-C04E-4E51-83B3-B562F9D263F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7250D12B-CB09-4793-9ACF-1E042C930405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="204">
   <si>
     <t>int</t>
   </si>
@@ -768,6 +768,14 @@
   </si>
   <si>
     <t>지속 방어도 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy_all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적 전체</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1210,11 +1218,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+      <pane ySplit="3" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2380,7 +2388,7 @@
         <v>119</v>
       </c>
       <c r="C70" s="1" t="str">
-        <f t="shared" ref="C70" si="4">UPPER(A70)&amp;"_"&amp;UPPER(B70)</f>
+        <f t="shared" ref="C70:C71" si="4">UPPER(A70)&amp;"_"&amp;UPPER(B70)</f>
         <v>TARGET_TYPE_ALLY_HP_LOWEST</v>
       </c>
       <c r="D70" s="3">
@@ -2390,67 +2398,67 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C71" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>TARGET_TYPE_ENEMY_ALL</v>
+      </c>
+      <c r="D71" s="3">
+        <v>4</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C72" s="1" t="str">
-        <f t="shared" ref="C72:C75" si="5">UPPER(A72)&amp;"_"&amp;UPPER(B72)</f>
-        <v>ACTIVE_CONDITION_BATTLE_START</v>
-      </c>
-      <c r="D72" s="3">
-        <v>0</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>182</v>
-      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" s="1" t="str">
+        <f t="shared" ref="C73:C76" si="5">UPPER(A73)&amp;"_"&amp;UPPER(B73)</f>
+        <v>ACTIVE_CONDITION_BATTLE_START</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C73" s="1" t="str">
+      <c r="C74" s="1" t="str">
         <f t="shared" si="5"/>
         <v>ACTIVE_CONDITION_BATTLE_END</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D74" s="3">
         <v>1</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C74" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>ACTIVE_CONDITION_HP_MINUS_VALUE</v>
-      </c>
-      <c r="D74" s="3">
-        <v>2</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2458,107 +2466,107 @@
         <v>168</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>ACTIVE_CONDITION_HP_MINUS_VALUE</v>
+      </c>
+      <c r="D75" s="3">
+        <v>2</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>ACTIVE_CONDITION_HP_PERCENT</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D76" s="3">
         <v>3</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+    <row r="77" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C77" s="1" t="str">
-        <f t="shared" ref="C77:C78" si="6">UPPER(A77)&amp;"_"&amp;UPPER(B77)</f>
-        <v>RELIC_EFFECT_HEAL</v>
-      </c>
-      <c r="D77" s="3">
-        <v>0</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>180</v>
-      </c>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="1" t="str">
+        <f t="shared" ref="C78:C79" si="6">UPPER(A78)&amp;"_"&amp;UPPER(B78)</f>
+        <v>RELIC_EFFECT_HEAL</v>
+      </c>
+      <c r="D78" s="3">
+        <v>0</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C78" s="1" t="str">
+      <c r="C79" s="1" t="str">
         <f t="shared" si="6"/>
         <v>RELIC_EFFECT_ARMOR</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D79" s="3">
         <v>1</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+    <row r="80" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C80" s="1" t="str">
-        <f t="shared" ref="C80:C84" si="7">UPPER(A80)&amp;"_"&amp;UPPER(B80)</f>
-        <v>MAP_TYPE_BATTLE_NORMAL</v>
-      </c>
-      <c r="D80" s="3">
-        <v>0</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C81" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>MAP_TYPE_BATTLE_ELITE</v>
+        <f t="shared" ref="C81:C85" si="7">UPPER(A81)&amp;"_"&amp;UPPER(B81)</f>
+        <v>MAP_TYPE_BATTLE_NORMAL</v>
       </c>
       <c r="D81" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2566,17 +2574,17 @@
         <v>126</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>MAP_TYPE_BATTLE_BOSS</v>
+        <v>MAP_TYPE_BATTLE_ELITE</v>
       </c>
       <c r="D82" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2584,17 +2592,17 @@
         <v>126</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C83" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>MAP_TYPE_SHOP</v>
+        <v>MAP_TYPE_BATTLE_BOSS</v>
       </c>
       <c r="D83" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2602,62 +2610,62 @@
         <v>126</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C84" s="1" t="str">
         <f t="shared" si="7"/>
+        <v>MAP_TYPE_SHOP</v>
+      </c>
+      <c r="D84" s="3">
+        <v>3</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>MAP_TYPE_ENHANCE</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D85" s="3">
         <v>4</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+    <row r="86" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C86" s="1" t="str">
-        <f t="shared" ref="C86:C101" si="8">UPPER(A86)&amp;"_"&amp;UPPER(B86)</f>
-        <v>REWARD_TYPE_ITEM</v>
-      </c>
-      <c r="D86" s="3">
-        <v>0</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C87" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>REWARD_TYPE_SPELL_SOURCE</v>
+        <f t="shared" ref="C87:C102" si="8">UPPER(A87)&amp;"_"&amp;UPPER(B87)</f>
+        <v>REWARD_TYPE_ITEM</v>
       </c>
       <c r="D87" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2665,17 +2673,17 @@
         <v>149</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C88" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>REWARD_TYPE_SUPPORT_MODULE</v>
+        <v>REWARD_TYPE_SPELL_SOURCE</v>
       </c>
       <c r="D88" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2683,62 +2691,62 @@
         <v>149</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="C89" s="1" t="str">
         <f t="shared" si="8"/>
+        <v>REWARD_TYPE_SUPPORT_MODULE</v>
+      </c>
+      <c r="D89" s="3">
+        <v>2</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C90" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>REWARD_TYPE_MONEY</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D90" s="3">
         <v>3</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+    <row r="91" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C91" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>EXCEPTION_TYPE_OWN_SPELL_SOURCE</v>
-      </c>
-      <c r="D91" s="3">
-        <v>0</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>159</v>
-      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C92" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>EXCEPTION_TYPE_NO_SPELL_SOURCE</v>
+        <v>EXCEPTION_TYPE_OWN_SPELL_SOURCE</v>
       </c>
       <c r="D92" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2746,17 +2754,17 @@
         <v>157</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C93" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>EXCEPTION_TYPE_CLEAR_MAP</v>
+        <v>EXCEPTION_TYPE_NO_SPELL_SOURCE</v>
       </c>
       <c r="D93" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2764,62 +2772,62 @@
         <v>157</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C94" s="1" t="str">
         <f t="shared" si="8"/>
+        <v>EXCEPTION_TYPE_CLEAR_MAP</v>
+      </c>
+      <c r="D94" s="3">
+        <v>2</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C95" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>EXCEPTION_TYPE_NOT_CLEAR_MAP</v>
       </c>
-      <c r="D94" s="3">
+      <c r="D95" s="3">
         <v>3</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+    <row r="96" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C96" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>RARITY_NORMAL</v>
-      </c>
-      <c r="D96" s="3">
-        <v>0</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>193</v>
-      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C97" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>RARITY_RARE</v>
+        <v>RARITY_NORMAL</v>
       </c>
       <c r="D97" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -2827,61 +2835,79 @@
         <v>189</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C98" s="1" t="str">
         <f t="shared" si="8"/>
+        <v>RARITY_RARE</v>
+      </c>
+      <c r="D98" s="3">
+        <v>1</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C99" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>RARITY_EPIC</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D99" s="3">
         <v>2</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+    <row r="100" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C100" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>LOGICAL_OPERATOR_AND</v>
-      </c>
-      <c r="D100" s="3">
-        <v>0</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C101" s="1" t="str">
         <f t="shared" si="8"/>
+        <v>LOGICAL_OPERATOR_AND</v>
+      </c>
+      <c r="D101" s="3">
+        <v>0</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C102" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>LOGICAL_OPERATOR_OR</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D102" s="3">
         <v>1</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[yerim]  support module 에 누락된 get_reward 구현
</commit_message>
<xml_diff>
--- a/GameData/Excel/enum.xlsx
+++ b/GameData/Excel/enum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yerim\portfolio_Game\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CD2095-DAFC-4609-B0CD-15DC26A15202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69BED26-6CA7-483E-B9A8-528072969C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="255">
   <si>
     <t>int</t>
   </si>
@@ -940,6 +940,14 @@
   </si>
   <si>
     <t>spell_source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보상 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_reward</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1385,11 +1393,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
+      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2556,49 +2564,49 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C70" s="1" t="str">
+        <f>UPPER(A70)&amp;"_"&amp;UPPER(B70)</f>
+        <v>SUPPORT_MODULE_EFFECT_GET_REWARD</v>
+      </c>
+      <c r="D70" s="3">
+        <v>5</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" s="1" t="str">
-        <f t="shared" ref="C71:C76" si="5">UPPER(A71)&amp;"_"&amp;UPPER(B71)</f>
-        <v>TARGET_TYPE_SELF</v>
-      </c>
-      <c r="D71" s="3">
-        <v>0</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="C72" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>TARGET_TYPE_ENEMY</v>
+        <f t="shared" ref="C72:C77" si="5">UPPER(A72)&amp;"_"&amp;UPPER(B72)</f>
+        <v>TARGET_TYPE_SELF</v>
       </c>
       <c r="D72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2606,17 +2614,17 @@
         <v>62</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C73" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>TARGET_TYPE_ALLY_HP_HIGHEST</v>
+        <v>TARGET_TYPE_ENEMY</v>
       </c>
       <c r="D73" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2624,17 +2632,17 @@
         <v>62</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C74" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>TARGET_TYPE_ALLY_HP_LOWEST</v>
+        <v>TARGET_TYPE_ALLY_HP_HIGHEST</v>
       </c>
       <c r="D74" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2642,17 +2650,17 @@
         <v>62</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>182</v>
+        <v>101</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>TARGET_TYPE_ENEMY_ALL</v>
+        <v>TARGET_TYPE_ALLY_HP_LOWEST</v>
       </c>
       <c r="D75" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2660,80 +2668,80 @@
         <v>62</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>241</v>
+        <v>182</v>
       </c>
       <c r="C76" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>TARGET_TYPE_ENEMY_ALL</v>
+      </c>
+      <c r="D76" s="3">
+        <v>4</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C77" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>TARGET_TYPE_ALLY_ALL</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D77" s="3">
         <v>5</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+    <row r="78" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C78" s="1" t="str">
-        <f>UPPER(A78)&amp;"_"&amp;UPPER(B78)</f>
-        <v>ACTIVE_CONDITION_BATTLE_START</v>
-      </c>
-      <c r="D78" s="3">
-        <v>0</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>163</v>
-      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C79" s="1" t="str">
         <f>UPPER(A79)&amp;"_"&amp;UPPER(B79)</f>
-        <v>ACTIVE_CONDITION_BATTLE_END</v>
+        <v>ACTIVE_CONDITION_BATTLE_START</v>
       </c>
       <c r="D79" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C80" s="1" t="str">
         <f>UPPER(A80)&amp;"_"&amp;UPPER(B80)</f>
-        <v>ACTIVE_CONDITION_HP_MINUS_VALUE</v>
+        <v>ACTIVE_CONDITION_BATTLE_END</v>
       </c>
       <c r="D80" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2741,107 +2749,107 @@
         <v>149</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C81" s="1" t="str">
         <f>UPPER(A81)&amp;"_"&amp;UPPER(B81)</f>
+        <v>ACTIVE_CONDITION_HP_MINUS_VALUE</v>
+      </c>
+      <c r="D81" s="3">
+        <v>2</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" s="1" t="str">
+        <f>UPPER(A82)&amp;"_"&amp;UPPER(B82)</f>
         <v>ACTIVE_CONDITION_HP_PERCENT</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D82" s="3">
         <v>3</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="83" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C83" s="1" t="str">
-        <f>UPPER(A83)&amp;"_"&amp;UPPER(B83)</f>
-        <v>RELIC_EFFECT_HEAL</v>
-      </c>
-      <c r="D83" s="3">
-        <v>0</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>161</v>
-      </c>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C84" s="1" t="str">
         <f>UPPER(A84)&amp;"_"&amp;UPPER(B84)</f>
+        <v>RELIC_EFFECT_HEAL</v>
+      </c>
+      <c r="D84" s="3">
+        <v>0</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C85" s="1" t="str">
+        <f>UPPER(A85)&amp;"_"&amp;UPPER(B85)</f>
         <v>RELIC_EFFECT_ARMOR</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D85" s="3">
         <v>1</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+    <row r="86" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C86" s="1" t="str">
-        <f t="shared" ref="C86:C91" si="6">UPPER(A86)&amp;"_"&amp;UPPER(B86)</f>
-        <v>MAP_TYPE_BATTLE_NORMAL</v>
-      </c>
-      <c r="D86" s="3">
-        <v>0</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C87" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>MAP_TYPE_BATTLE_ELITE</v>
+        <f t="shared" ref="C87:C92" si="6">UPPER(A87)&amp;"_"&amp;UPPER(B87)</f>
+        <v>MAP_TYPE_BATTLE_NORMAL</v>
       </c>
       <c r="D87" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2849,17 +2857,17 @@
         <v>108</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C88" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>MAP_TYPE_BATTLE_BOSS</v>
+        <v>MAP_TYPE_BATTLE_ELITE</v>
       </c>
       <c r="D88" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2867,17 +2875,17 @@
         <v>108</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C89" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>MAP_TYPE_SHOP</v>
+        <v>MAP_TYPE_BATTLE_BOSS</v>
       </c>
       <c r="D89" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2885,17 +2893,17 @@
         <v>108</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C90" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>MAP_TYPE_ENHANCE</v>
+        <v>MAP_TYPE_SHOP</v>
       </c>
       <c r="D90" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2903,62 +2911,62 @@
         <v>108</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
       <c r="C91" s="1" t="str">
         <f t="shared" si="6"/>
+        <v>MAP_TYPE_ENHANCE</v>
+      </c>
+      <c r="D91" s="3">
+        <v>4</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>MAP_TYPE_SPECIAL</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D92" s="3">
         <v>5</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+    <row r="93" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C93" s="1" t="str">
-        <f>UPPER(A93)&amp;"_"&amp;UPPER(B93)</f>
-        <v>REWARD_TYPE_ITEM</v>
-      </c>
-      <c r="D93" s="3">
-        <v>0</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>252</v>
+        <v>132</v>
       </c>
       <c r="C94" s="1" t="str">
         <f>UPPER(A94)&amp;"_"&amp;UPPER(B94)</f>
-        <v>REWARD_TYPE_SPELL_SOURCE</v>
+        <v>REWARD_TYPE_ITEM</v>
       </c>
       <c r="D94" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2966,17 +2974,17 @@
         <v>131</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="C95" s="1" t="str">
         <f>UPPER(A95)&amp;"_"&amp;UPPER(B95)</f>
-        <v>REWARD_TYPE_SUPPORT_MODULE</v>
+        <v>REWARD_TYPE_SPELL_SOURCE</v>
       </c>
       <c r="D95" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2984,17 +2992,17 @@
         <v>131</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="C96" s="1" t="str">
         <f>UPPER(A96)&amp;"_"&amp;UPPER(B96)</f>
-        <v>REWARD_TYPE_MONEY</v>
+        <v>REWARD_TYPE_SUPPORT_MODULE</v>
       </c>
       <c r="D96" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3002,62 +3010,62 @@
         <v>131</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>251</v>
+        <v>179</v>
       </c>
       <c r="C97" s="1" t="str">
         <f>UPPER(A97)&amp;"_"&amp;UPPER(B97)</f>
+        <v>REWARD_TYPE_MONEY</v>
+      </c>
+      <c r="D97" s="3">
+        <v>3</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C98" s="1" t="str">
+        <f>UPPER(A98)&amp;"_"&amp;UPPER(B98)</f>
         <v>REWARD_TYPE_SPELL_COMBINE</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D98" s="3">
         <v>4</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
+    <row r="99" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C99" s="1" t="str">
-        <f>UPPER(A99)&amp;"_"&amp;UPPER(B99)</f>
-        <v>EXCEPTION_TYPE_OWN_SPELL_SOURCE</v>
-      </c>
-      <c r="D99" s="3">
-        <v>0</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C100" s="1" t="str">
         <f>UPPER(A100)&amp;"_"&amp;UPPER(B100)</f>
-        <v>EXCEPTION_TYPE_NO_SPELL_SOURCE</v>
+        <v>EXCEPTION_TYPE_OWN_SPELL_SOURCE</v>
       </c>
       <c r="D100" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3065,17 +3073,17 @@
         <v>138</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C101" s="1" t="str">
         <f>UPPER(A101)&amp;"_"&amp;UPPER(B101)</f>
-        <v>EXCEPTION_TYPE_CLEAR_MAP</v>
+        <v>EXCEPTION_TYPE_NO_SPELL_SOURCE</v>
       </c>
       <c r="D101" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -3083,62 +3091,62 @@
         <v>138</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C102" s="1" t="str">
         <f>UPPER(A102)&amp;"_"&amp;UPPER(B102)</f>
+        <v>EXCEPTION_TYPE_CLEAR_MAP</v>
+      </c>
+      <c r="D102" s="3">
+        <v>2</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C103" s="1" t="str">
+        <f>UPPER(A103)&amp;"_"&amp;UPPER(B103)</f>
         <v>EXCEPTION_TYPE_NOT_CLEAR_MAP</v>
       </c>
-      <c r="D102" s="3">
+      <c r="D103" s="3">
         <v>3</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
+    <row r="104" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C104" s="1" t="str">
-        <f>UPPER(A104)&amp;"_"&amp;UPPER(B104)</f>
-        <v>RARITY_NORMAL</v>
-      </c>
-      <c r="D104" s="3">
-        <v>0</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C105" s="1" t="str">
         <f>UPPER(A105)&amp;"_"&amp;UPPER(B105)</f>
-        <v>RARITY_RARE</v>
+        <v>RARITY_NORMAL</v>
       </c>
       <c r="D105" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -3146,107 +3154,107 @@
         <v>170</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C106" s="1" t="str">
         <f>UPPER(A106)&amp;"_"&amp;UPPER(B106)</f>
+        <v>RARITY_RARE</v>
+      </c>
+      <c r="D106" s="3">
+        <v>1</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C107" s="1" t="str">
+        <f>UPPER(A107)&amp;"_"&amp;UPPER(B107)</f>
         <v>RARITY_EPIC</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D107" s="3">
         <v>2</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+    <row r="108" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C108" s="1" t="str">
-        <f>UPPER(A108)&amp;"_"&amp;UPPER(B108)</f>
-        <v>LOGICAL_OPERATOR_AND</v>
-      </c>
-      <c r="D108" s="3">
-        <v>0</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>155</v>
-      </c>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C109" s="1" t="str">
         <f>UPPER(A109)&amp;"_"&amp;UPPER(B109)</f>
+        <v>LOGICAL_OPERATOR_AND</v>
+      </c>
+      <c r="D109" s="3">
+        <v>0</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C110" s="1" t="str">
+        <f>UPPER(A110)&amp;"_"&amp;UPPER(B110)</f>
         <v>LOGICAL_OPERATOR_OR</v>
       </c>
-      <c r="D109" s="3">
+      <c r="D110" s="3">
         <v>1</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E110" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+    <row r="111" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C111" s="1" t="str">
-        <f>UPPER(A111)&amp;"_"&amp;UPPER(B111)</f>
-        <v>DIALOG_TYPE_TITLE</v>
-      </c>
-      <c r="D111" s="3">
-        <v>0</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C112" s="1" t="str">
         <f>UPPER(A112)&amp;"_"&amp;UPPER(B112)</f>
-        <v>DIALOG_TYPE_TEXT</v>
+        <v>DIALOG_TYPE_TITLE</v>
       </c>
       <c r="D112" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -3254,62 +3262,62 @@
         <v>190</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C113" s="1" t="str">
         <f>UPPER(A113)&amp;"_"&amp;UPPER(B113)</f>
+        <v>DIALOG_TYPE_TEXT</v>
+      </c>
+      <c r="D113" s="3">
+        <v>1</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C114" s="1" t="str">
+        <f>UPPER(A114)&amp;"_"&amp;UPPER(B114)</f>
         <v>DIALOG_TYPE_BUTTON</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D114" s="3">
         <v>2</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E114" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+    <row r="115" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C115" s="1" t="str">
-        <f t="shared" ref="C115:C123" si="7">UPPER(A115)&amp;"_"&amp;UPPER(B115)</f>
-        <v>BUTTON_FUNCTION_REWARD</v>
-      </c>
-      <c r="D115" s="3">
-        <v>0</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>199</v>
-      </c>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C116" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_SELECT_REWARD</v>
+        <f t="shared" ref="C116:C124" si="7">UPPER(A116)&amp;"_"&amp;UPPER(B116)</f>
+        <v>BUTTON_FUNCTION_REWARD</v>
       </c>
       <c r="D116" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -3317,17 +3325,17 @@
         <v>197</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C117" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_DELETE_SOURCE</v>
+        <v>BUTTON_FUNCTION_SELECT_REWARD</v>
       </c>
       <c r="D117" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3335,17 +3343,17 @@
         <v>197</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C118" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_DELETE_SUPPORT_MODULE</v>
+        <v>BUTTON_FUNCTION_DELETE_SOURCE</v>
       </c>
       <c r="D118" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3353,17 +3361,17 @@
         <v>197</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C119" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_DELETE_RELIC</v>
+        <v>BUTTON_FUNCTION_DELETE_SUPPORT_MODULE</v>
       </c>
       <c r="D119" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3371,17 +3379,17 @@
         <v>197</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C120" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_SHOP</v>
+        <v>BUTTON_FUNCTION_DELETE_RELIC</v>
       </c>
       <c r="D120" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3389,17 +3397,17 @@
         <v>197</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C121" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_ENHANCE</v>
+        <v>BUTTON_FUNCTION_SHOP</v>
       </c>
       <c r="D121" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -3407,17 +3415,17 @@
         <v>197</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C122" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>BUTTON_FUNCTION_EXCHANGE</v>
+        <v>BUTTON_FUNCTION_ENHANCE</v>
       </c>
       <c r="D122" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -3425,62 +3433,62 @@
         <v>197</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C123" s="1" t="str">
         <f t="shared" si="7"/>
+        <v>BUTTON_FUNCTION_EXCHANGE</v>
+      </c>
+      <c r="D123" s="3">
+        <v>7</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C124" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>BUTTON_FUNCTION_EXIT</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D124" s="3">
         <v>8</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="E124" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
+    <row r="125" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C125" s="1" t="str">
-        <f>UPPER(A125)&amp;"_"&amp;UPPER(B125)</f>
-        <v>ITEM_TYPE_SOURCE</v>
-      </c>
-      <c r="D125" s="3">
-        <v>0</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>219</v>
-      </c>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>135</v>
+        <v>218</v>
       </c>
       <c r="C126" s="1" t="str">
         <f>UPPER(A126)&amp;"_"&amp;UPPER(B126)</f>
-        <v>ITEM_TYPE_SUPPORT_MODULE</v>
+        <v>ITEM_TYPE_SOURCE</v>
       </c>
       <c r="D126" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -3488,16 +3496,34 @@
         <v>217</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>221</v>
+        <v>135</v>
       </c>
       <c r="C127" s="1" t="str">
         <f>UPPER(A127)&amp;"_"&amp;UPPER(B127)</f>
+        <v>ITEM_TYPE_SUPPORT_MODULE</v>
+      </c>
+      <c r="D127" s="3">
+        <v>1</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C128" s="1" t="str">
+        <f>UPPER(A128)&amp;"_"&amp;UPPER(B128)</f>
         <v>ITEM_TYPE_RELIC</v>
       </c>
-      <c r="D127" s="3">
+      <c r="D128" s="3">
         <v>2</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E128" s="3" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>